<commit_message>
chore: update user management logic and improve import functionality
</commit_message>
<xml_diff>
--- a/public/Medvanta - Bulk User Template.xlsx
+++ b/public/Medvanta - Bulk User Template.xlsx
@@ -11,21 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">User assignment template for the VantaVerse app. </t>
   </si>
   <si>
-    <t>1. Organizations &amp; Teams match by name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Teams must have an organization field. </t>
-  </si>
-  <si>
-    <t>3. Email is the only required field.</t>
-  </si>
-  <si>
-    <t>4. If a user already exists, they will be assigned to the organization/team.</t>
+    <t>Email is the only required field.</t>
   </si>
   <si>
     <t>First Name</t>
@@ -35,15 +26,6 @@
   </si>
   <si>
     <t>Email*</t>
-  </si>
-  <si>
-    <t>Organization Name (exact)</t>
-  </si>
-  <si>
-    <t>Team Name (exact, must have organization)</t>
-  </si>
-  <si>
-    <t>Role (admin or user)</t>
   </si>
 </sst>
 </file>
@@ -95,7 +77,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -105,9 +87,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -422,7 +401,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -453,162 +432,38 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>